<commit_message>
subo completo el excel con el diccionario de datos del taller
</commit_message>
<xml_diff>
--- a/EntregaTalleres/Taller_Repaso_Bases_Datos.xlsx
+++ b/EntregaTalleres/Taller_Repaso_Bases_Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamour\Documents\GitHub\TrabajoIndividual\EntregaTalleres\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cba425722e35f70/Documentos/GitHub/TrabajoIndividual/EntregaTalleres/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65E0B402-EA43-41D5-84DE-41F9E4664DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02B8D0BB-0E61-48C9-9856-8DF159FB9DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{60A5F529-99B0-4822-BC8A-4F95BCD50130}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{60A5F529-99B0-4822-BC8A-4F95BCD50130}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="220">
   <si>
     <t>idVotacion</t>
   </si>
@@ -518,9 +518,6 @@
     <t xml:space="preserve"> nomJornada</t>
   </si>
   <si>
-    <t>EstadoJ</t>
-  </si>
-  <si>
     <t>Llave primaria con id auto incrementable de la jornada</t>
   </si>
   <si>
@@ -548,9 +545,6 @@
     <t xml:space="preserve"> nomGenero</t>
   </si>
   <si>
-    <t>EstadoG</t>
-  </si>
-  <si>
     <t>Llave primaria con id auto incrementable del genero</t>
   </si>
   <si>
@@ -563,9 +557,6 @@
     <t xml:space="preserve"> nomTipoDoc</t>
   </si>
   <si>
-    <t>EstadoTD</t>
-  </si>
-  <si>
     <t>Llave primaria con id auto incrementable del tipo de documento</t>
   </si>
   <si>
@@ -581,9 +572,6 @@
     <t xml:space="preserve"> nomTipoMiembro</t>
   </si>
   <si>
-    <t>EstadoTM</t>
-  </si>
-  <si>
     <t>Llave primaria con id auto incrementable del tipo de miembro</t>
   </si>
   <si>
@@ -602,10 +590,112 @@
     <t xml:space="preserve"> nomCurso</t>
   </si>
   <si>
-    <t>EstadoCu</t>
-  </si>
-  <si>
     <t>Llave primaria con id auto incrementable del curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nomConcejo</t>
+  </si>
+  <si>
+    <t>Llave primaria con id auto incrementable del concejo</t>
+  </si>
+  <si>
+    <t>Nombre del concejo</t>
+  </si>
+  <si>
+    <t>Estado del concejo</t>
+  </si>
+  <si>
+    <t>Tabla que contiene los datos del concejo</t>
+  </si>
+  <si>
+    <t>Concejo</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Tabla que contiene los datos del cargo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nomCargo</t>
+  </si>
+  <si>
+    <t>idConcejoFK</t>
+  </si>
+  <si>
+    <t>Llave foranea del id el concejo correspondiente al cargo</t>
+  </si>
+  <si>
+    <t>Foreign key, Not null</t>
+  </si>
+  <si>
+    <t>Tabla que contiene los datos de la elección</t>
+  </si>
+  <si>
+    <t>Llave primaria con id auto incrementable de la eleccion</t>
+  </si>
+  <si>
+    <t>Año de la eleccion</t>
+  </si>
+  <si>
+    <t>Fecha de la eleccion en formato 00-00-0000</t>
+  </si>
+  <si>
+    <t>Estado de la eleccion</t>
+  </si>
+  <si>
+    <t>Votacion</t>
+  </si>
+  <si>
+    <t>Eleccion</t>
+  </si>
+  <si>
+    <t>Tabla que contiene los datos de la votacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idUsuarioVotanteFK</t>
+  </si>
+  <si>
+    <t>Llave primaria con id auto incrementable de la votación</t>
+  </si>
+  <si>
+    <t>Hora de votacion en formato 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llave foranea del id del usuario votante </t>
+  </si>
+  <si>
+    <t>Llave foranea del id del post candidato</t>
+  </si>
+  <si>
+    <t>Estado de la votacióon</t>
+  </si>
+  <si>
+    <t>Postulacion_candidato</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idEleccionFK</t>
+  </si>
+  <si>
+    <t>idCargoFK</t>
+  </si>
+  <si>
+    <t>Estado del candidato</t>
+  </si>
+  <si>
+    <t>Número total de votos</t>
+  </si>
+  <si>
+    <t>Propuestas del candidato</t>
+  </si>
+  <si>
+    <t>Llave foranea del id del cargo</t>
+  </si>
+  <si>
+    <t>Llave foranea del id de la elección</t>
+  </si>
+  <si>
+    <t>Llave foranea del id del usuario</t>
   </si>
 </sst>
 </file>
@@ -722,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -756,6 +846,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,13 +888,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -794,6 +896,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +936,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>773748</xdr:colOff>
+      <xdr:colOff>501604</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
@@ -873,9 +981,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -913,7 +1021,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1019,7 +1127,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1161,7 +1269,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1174,8 +1282,8 @@
   </sheetPr>
   <dimension ref="B1:X39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L13"/>
+    <sheetView topLeftCell="J18" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1293,7 @@
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
@@ -1204,33 +1312,33 @@
   <sheetData>
     <row r="1" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:24" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="F2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
       <c r="J2"/>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="15"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="21"/>
     </row>
     <row r="3" spans="2:24" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1472,11 +1580,11 @@
       </c>
     </row>
     <row r="7" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
       <c r="F7" s="2">
         <v>4</v>
       </c>
@@ -1822,16 +1930,16 @@
       </c>
     </row>
     <row r="13" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="F13" s="13" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="F13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
       <c r="K13" s="2">
         <v>10</v>
       </c>
@@ -1928,13 +2036,13 @@
       <c r="H15" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
@@ -2042,12 +2150,12 @@
       <c r="D19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
       <c r="K19" s="2">
         <v>3</v>
       </c>
@@ -2097,11 +2205,11 @@
       </c>
     </row>
     <row r="21" spans="2:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
@@ -2242,12 +2350,12 @@
       <c r="D25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
       <c r="K25" s="2">
         <v>9</v>
       </c>
@@ -2323,15 +2431,15 @@
       <c r="I28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="15"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="21"/>
     </row>
     <row r="29" spans="2:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="2">
@@ -2470,17 +2578,17 @@
     <row r="39" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="K2:X2"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="K28:Q28"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="K15:O15"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2488,22 +2596,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C2D30D-7D44-4709-A21F-12E8DD6CA189}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" customWidth="1"/>
     <col min="17" max="17" width="19.140625" customWidth="1"/>
   </cols>
@@ -2512,88 +2622,88 @@
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="G1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
       <c r="M1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="19"/>
+      <c r="N1" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="26">
         <v>45747</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
       <c r="G2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="26">
         <v>45747</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="25"/>
       <c r="M2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="20">
+      <c r="N2" s="26">
         <v>45747</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="19"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="25"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
       <c r="G3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="19"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
       <c r="M3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="19"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="1:17" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -2643,7 +2753,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -2654,37 +2764,37 @@
         <v>138</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G5" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="2" t="s">
         <v>138</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="M5" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="O5" s="22"/>
+      <c r="O5" s="17"/>
       <c r="P5" s="2" t="s">
         <v>138</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -2697,39 +2807,39 @@
       <c r="E6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="I6" s="22">
+      <c r="H6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="17">
         <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>140</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="N6" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="O6" s="22">
+      <c r="M6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O6" s="17">
         <v>10</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>140</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -2742,39 +2852,39 @@
       <c r="E7" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="I7" s="22">
+      <c r="G7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="17">
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>140</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="O7" s="22">
+        <v>164</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O7" s="17">
         <v>5</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>140</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -2789,14 +2899,14 @@
       <c r="E8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -2811,14 +2921,14 @@
       <c r="E9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -2834,24 +2944,24 @@
       <c r="G10" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="H10" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
       <c r="M10" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="19"/>
+      <c r="N10" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -2869,24 +2979,24 @@
       <c r="G11" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="26">
         <v>45747</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
       <c r="M11" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="26">
         <v>45747</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -2904,24 +3014,24 @@
       <c r="G12" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="H12" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
       <c r="M12" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="19"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -2968,11 +3078,11 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="11">
         <v>10</v>
@@ -2983,35 +3093,35 @@
       <c r="E14" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="I14" s="22"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="2" t="s">
         <v>138</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="M14" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="M14" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="22" t="s">
+      <c r="N14" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="O14" s="22"/>
+      <c r="O14" s="17"/>
       <c r="P14" s="2" t="s">
         <v>138</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -3024,39 +3134,39 @@
       <c r="E15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="I15" s="22">
+      <c r="G15" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I15" s="17">
         <v>10</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>140</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="N15" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="O15" s="22">
+        <v>170</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O15" s="17">
         <v>10</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>140</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="9" t="s">
         <v>121</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -3069,39 +3179,39 @@
       <c r="E16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="I16" s="22">
+      <c r="G16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" s="17">
         <v>5</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>140</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="N16" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="O16" s="22">
+        <v>164</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O16" s="17">
         <v>5</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>140</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -3114,14 +3224,14 @@
       <c r="E17" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>123</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -3136,46 +3246,100 @@
       <c r="E18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="G20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="25"/>
+      <c r="M20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="N20" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="25"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="26">
         <v>45747</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="G21" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="26">
+        <v>45747</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="25"/>
+      <c r="M21" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" s="26">
+        <v>45747</v>
+      </c>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="25"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="G22" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="25"/>
+      <c r="M22" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="25"/>
+    </row>
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>128</v>
       </c>
@@ -3191,58 +3355,637 @@
       <c r="E23" s="9" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="G23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" s="22">
+        <v>184</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="17">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B26" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="C26" s="22">
+      <c r="G25" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" s="17">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O25" s="17">
+        <v>10</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="17">
         <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" s="17">
+        <v>5</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O26" s="17">
+        <v>5</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="O27" s="17">
+        <v>5</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="G29" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="25"/>
+      <c r="M29" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="N29" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="25"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="16">
+        <v>45747</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="26">
+        <v>45747</v>
+      </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="25"/>
+      <c r="M30" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N30" s="26">
+        <v>45747</v>
+      </c>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="25"/>
+    </row>
+    <row r="31" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="G31" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
+      <c r="M31" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="N31" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="25"/>
+    </row>
+    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q32" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O33" s="17"/>
+      <c r="P33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="17">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I34" s="17">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="O34" s="17">
+        <v>10</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="17">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="17"/>
+      <c r="J35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O35" s="17"/>
+      <c r="P35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="17">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O36" s="17"/>
+      <c r="P36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G37" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I37" s="17">
+        <v>10</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="O37" s="17">
+        <v>50</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="M38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O38" s="17"/>
+      <c r="P38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G39" s="27"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="M39" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="O39" s="17">
+        <v>10</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G40" s="27"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G41" s="27"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G42" s="27"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G43" s="27"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G44" s="27"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G45" s="27"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G46" s="27"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="31">
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
@@ -3259,8 +4002,6 @@
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>